<commit_message>
sửa lại template của báo cáo thay đổi trạng thái store
</commit_message>
<xml_diff>
--- a/DMS/Templates/Report_Store_State_Change.xlsx
+++ b/DMS/Templates/Report_Store_State_Change.xlsx
@@ -104,13 +104,13 @@
     <t>{{ReportStoreStateChange.Details.PreviousStoreStatus}}</t>
   </si>
   <si>
-    <t>{{ReportStoreStateChange.StringCreatedAt}}</t>
-  </si>
-  <si>
     <t>{{ReportStoreStateChange.Details.StorePhoneNumber}}</t>
   </si>
   <si>
-    <t>{{ReportStoreStateChange.Stt}}</t>
+    <t>{{ReportStoreStateChange.Details.StringCreatedAt}}</t>
+  </si>
+  <si>
+    <t>{{ReportStoreStateChange.Details.Stt}}</t>
   </si>
 </sst>
 </file>
@@ -578,7 +578,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:H10"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -588,7 +588,7 @@
     <col min="3" max="3" width="16.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="33" style="1" customWidth="1"/>
     <col min="5" max="5" width="43.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="22.140625" style="1" customWidth="1"/>
     <col min="7" max="7" width="20.42578125" style="1" customWidth="1"/>
     <col min="8" max="8" width="15.5703125" style="1" customWidth="1"/>
     <col min="9" max="9" width="16" style="1" customWidth="1"/>
@@ -631,17 +631,16 @@
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5" t="s">
+      <c r="D5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="E5" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="F5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="G5" s="9" t="s">
         <v>15</v>
       </c>
     </row>
@@ -696,7 +695,7 @@
         <v>28</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>19</v>
@@ -708,7 +707,7 @@
         <v>22</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>25</v>

</xml_diff>